<commit_message>
Updated wing results for field
Sent to Giovan, still need to figure out shape
</commit_message>
<xml_diff>
--- a/popgen/2017_11_10 Pop Gen Full sample info.xlsx
+++ b/popgen/2017_11_10 Pop Gen Full sample info.xlsx
@@ -2579,14 +2579,14 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -13114,13 +13114,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ADAC7E-9BA3-4B3E-8573-611E72D1A3C2}">
   <dimension ref="A1:G190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="17.75" style="123" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="121" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -13410,7 +13410,7 @@
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="123" t="s">
+      <c r="C15" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E15" s="15" t="s">
@@ -13430,7 +13430,7 @@
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -13450,7 +13450,7 @@
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E17" s="15" t="s">
@@ -13470,7 +13470,7 @@
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="123" t="s">
+      <c r="C18" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -13490,7 +13490,7 @@
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="123" t="s">
+      <c r="C19" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E19" s="15" t="s">
@@ -13510,7 +13510,7 @@
       <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="123" t="s">
+      <c r="C20" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -13530,7 +13530,7 @@
       <c r="B21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="123" t="s">
+      <c r="C21" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E21" s="15" t="s">
@@ -13550,7 +13550,7 @@
       <c r="B22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="123" t="s">
+      <c r="C22" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -13570,7 +13570,7 @@
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -13590,7 +13590,7 @@
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E24" s="15" t="s">
@@ -13610,7 +13610,7 @@
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E25" s="15" t="s">
@@ -13630,7 +13630,7 @@
       <c r="B26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="123" t="s">
+      <c r="C26" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E26" s="15" t="s">
@@ -13650,7 +13650,7 @@
       <c r="B27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="123" t="s">
+      <c r="C27" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E27" s="15" t="s">
@@ -13670,7 +13670,7 @@
       <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="123" t="s">
+      <c r="C28" s="121" t="s">
         <v>651</v>
       </c>
       <c r="E28" s="15" t="s">
@@ -13690,7 +13690,7 @@
       <c r="B29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="123" t="s">
+      <c r="C29" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -13710,7 +13710,7 @@
       <c r="B30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="123" t="s">
+      <c r="C30" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E30" s="15" t="s">
@@ -13730,7 +13730,7 @@
       <c r="B31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="123" t="s">
+      <c r="C31" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E31" s="15" t="s">
@@ -13750,7 +13750,7 @@
       <c r="B32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="123" t="s">
+      <c r="C32" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E32" s="15" t="s">
@@ -13770,7 +13770,7 @@
       <c r="B33" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="123" t="s">
+      <c r="C33" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E33" s="15" t="s">
@@ -13790,7 +13790,7 @@
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="123" t="s">
+      <c r="C34" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E34" s="15" t="s">
@@ -13810,7 +13810,7 @@
       <c r="B35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="123" t="s">
+      <c r="C35" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E35" s="15" t="s">
@@ -13830,7 +13830,7 @@
       <c r="B36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="123" t="s">
+      <c r="C36" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E36" s="15" t="s">
@@ -13850,7 +13850,7 @@
       <c r="B37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="123" t="s">
+      <c r="C37" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E37" s="15" t="s">
@@ -13870,7 +13870,7 @@
       <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="123" t="s">
+      <c r="C38" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E38" s="15" t="s">
@@ -13890,7 +13890,7 @@
       <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E39" s="15" t="s">
@@ -13910,7 +13910,7 @@
       <c r="B40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="123" t="s">
+      <c r="C40" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E40" s="15" t="s">
@@ -13930,7 +13930,7 @@
       <c r="B41" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="123" t="s">
+      <c r="C41" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E41" s="15" t="s">
@@ -13950,7 +13950,7 @@
       <c r="B42" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="123" t="s">
+      <c r="C42" s="121" t="s">
         <v>652</v>
       </c>
       <c r="E42" s="15" t="s">
@@ -13970,7 +13970,7 @@
       <c r="B43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="123" t="s">
+      <c r="C43" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E43" s="15" t="s">
@@ -13990,7 +13990,7 @@
       <c r="B44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="123" t="s">
+      <c r="C44" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E44" s="15" t="s">
@@ -14010,7 +14010,7 @@
       <c r="B45" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="123" t="s">
+      <c r="C45" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E45" s="15" t="s">
@@ -14030,7 +14030,7 @@
       <c r="B46" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="123" t="s">
+      <c r="C46" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E46" s="15" t="s">
@@ -14050,7 +14050,7 @@
       <c r="B47" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="123" t="s">
+      <c r="C47" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E47" s="15" t="s">
@@ -14070,7 +14070,7 @@
       <c r="B48" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="123" t="s">
+      <c r="C48" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E48" s="15" t="s">
@@ -14090,7 +14090,7 @@
       <c r="B49" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="123" t="s">
+      <c r="C49" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E49" s="15" t="s">
@@ -14110,7 +14110,7 @@
       <c r="B50" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="123" t="s">
+      <c r="C50" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E50" s="15" t="s">
@@ -14130,7 +14130,7 @@
       <c r="B51" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="123" t="s">
+      <c r="C51" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E51" s="15" t="s">
@@ -14150,7 +14150,7 @@
       <c r="B52" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="123" t="s">
+      <c r="C52" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E52" s="15" t="s">
@@ -14170,7 +14170,7 @@
       <c r="B53" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="123" t="s">
+      <c r="C53" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E53" s="15" t="s">
@@ -14190,7 +14190,7 @@
       <c r="B54" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="123" t="s">
+      <c r="C54" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E54" s="15" t="s">
@@ -14210,7 +14210,7 @@
       <c r="B55" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="123" t="s">
+      <c r="C55" s="121" t="s">
         <v>653</v>
       </c>
       <c r="E55" s="15" t="s">
@@ -14230,7 +14230,7 @@
       <c r="B56" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="123" t="s">
+      <c r="C56" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E56" s="15" t="s">
@@ -14250,7 +14250,7 @@
       <c r="B57" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="123" t="s">
+      <c r="C57" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E57" s="15" t="s">
@@ -14270,7 +14270,7 @@
       <c r="B58" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="123" t="s">
+      <c r="C58" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E58" s="15" t="s">
@@ -14290,7 +14290,7 @@
       <c r="B59" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="123" t="s">
+      <c r="C59" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E59" s="15" t="s">
@@ -14310,7 +14310,7 @@
       <c r="B60" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="123" t="s">
+      <c r="C60" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E60" s="15" t="s">
@@ -14330,7 +14330,7 @@
       <c r="B61" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="123" t="s">
+      <c r="C61" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E61" s="15" t="s">
@@ -14350,7 +14350,7 @@
       <c r="B62" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="123" t="s">
+      <c r="C62" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E62" s="15" t="s">
@@ -14370,7 +14370,7 @@
       <c r="B63" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="123" t="s">
+      <c r="C63" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E63" s="15" t="s">
@@ -14390,7 +14390,7 @@
       <c r="B64" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="123" t="s">
+      <c r="C64" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E64" s="15" t="s">
@@ -14410,7 +14410,7 @@
       <c r="B65" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="123" t="s">
+      <c r="C65" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E65" s="15" t="s">
@@ -14430,7 +14430,7 @@
       <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="123" t="s">
+      <c r="C66" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E66" s="15" t="s">
@@ -14450,7 +14450,7 @@
       <c r="B67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="123" t="s">
+      <c r="C67" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E67" s="15" t="s">
@@ -14470,7 +14470,7 @@
       <c r="B68" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C68" s="123" t="s">
+      <c r="C68" s="121" t="s">
         <v>654</v>
       </c>
       <c r="E68" s="15" t="s">
@@ -14750,7 +14750,7 @@
       <c r="B82" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C82" s="123" t="s">
+      <c r="C82" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E82" s="4" t="s">
@@ -14770,7 +14770,7 @@
       <c r="B83" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="123" t="s">
+      <c r="C83" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E83" s="4" t="s">
@@ -14790,7 +14790,7 @@
       <c r="B84" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C84" s="123" t="s">
+      <c r="C84" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E84" s="4" t="s">
@@ -14810,7 +14810,7 @@
       <c r="B85" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="123" t="s">
+      <c r="C85" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E85" s="4" t="s">
@@ -14830,7 +14830,7 @@
       <c r="B86" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="123" t="s">
+      <c r="C86" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E86" s="4" t="s">
@@ -14850,7 +14850,7 @@
       <c r="B87" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="123" t="s">
+      <c r="C87" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E87" s="4" t="s">
@@ -14870,7 +14870,7 @@
       <c r="B88" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="123" t="s">
+      <c r="C88" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E88" s="4" t="s">
@@ -14890,7 +14890,7 @@
       <c r="B89" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="123" t="s">
+      <c r="C89" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E89" s="4" t="s">
@@ -14910,7 +14910,7 @@
       <c r="B90" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C90" s="123" t="s">
+      <c r="C90" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E90" s="4" t="s">
@@ -14930,7 +14930,7 @@
       <c r="B91" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C91" s="123" t="s">
+      <c r="C91" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E91" s="4" t="s">
@@ -14950,7 +14950,7 @@
       <c r="B92" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C92" s="123" t="s">
+      <c r="C92" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E92" s="4" t="s">
@@ -14970,7 +14970,7 @@
       <c r="B93" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C93" s="123" t="s">
+      <c r="C93" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E93" s="4" t="s">
@@ -14990,7 +14990,7 @@
       <c r="B94" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="123" t="s">
+      <c r="C94" s="121" t="s">
         <v>655</v>
       </c>
       <c r="E94" s="4" t="s">
@@ -15270,7 +15270,7 @@
       <c r="B108" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C108" s="123" t="s">
+      <c r="C108" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E108" s="15" t="s">
@@ -15290,7 +15290,7 @@
       <c r="B109" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C109" s="123" t="s">
+      <c r="C109" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E109" s="15" t="s">
@@ -15310,7 +15310,7 @@
       <c r="B110" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C110" s="123" t="s">
+      <c r="C110" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E110" s="15" t="s">
@@ -15330,7 +15330,7 @@
       <c r="B111" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C111" s="123" t="s">
+      <c r="C111" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E111" s="15" t="s">
@@ -15350,7 +15350,7 @@
       <c r="B112" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C112" s="123" t="s">
+      <c r="C112" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E112" s="15" t="s">
@@ -15370,7 +15370,7 @@
       <c r="B113" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="123" t="s">
+      <c r="C113" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E113" s="117" t="s">
@@ -15390,7 +15390,7 @@
       <c r="B114" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C114" s="123" t="s">
+      <c r="C114" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E114" s="15" t="s">
@@ -15410,7 +15410,7 @@
       <c r="B115" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C115" s="123" t="s">
+      <c r="C115" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E115" s="15" t="s">
@@ -15430,7 +15430,7 @@
       <c r="B116" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C116" s="123" t="s">
+      <c r="C116" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E116" s="15" t="s">
@@ -15450,7 +15450,7 @@
       <c r="B117" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C117" s="123" t="s">
+      <c r="C117" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E117" s="15" t="s">
@@ -15470,7 +15470,7 @@
       <c r="B118" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C118" s="123" t="s">
+      <c r="C118" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E118" s="15" t="s">
@@ -15490,7 +15490,7 @@
       <c r="B119" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C119" s="123" t="s">
+      <c r="C119" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E119" s="15" t="s">
@@ -15510,7 +15510,7 @@
       <c r="B120" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C120" s="123" t="s">
+      <c r="C120" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E120" s="15" t="s">
@@ -15530,7 +15530,7 @@
       <c r="B121" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C121" s="123" t="s">
+      <c r="C121" s="121" t="s">
         <v>656</v>
       </c>
       <c r="E121" s="15" t="s">
@@ -15550,7 +15550,7 @@
       <c r="B122" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C122" s="123" t="s">
+      <c r="C122" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E122" s="4" t="s">
@@ -15570,7 +15570,7 @@
       <c r="B123" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C123" s="123" t="s">
+      <c r="C123" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E123" s="4" t="s">
@@ -15590,7 +15590,7 @@
       <c r="B124" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C124" s="123" t="s">
+      <c r="C124" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E124" s="4" t="s">
@@ -15610,7 +15610,7 @@
       <c r="B125" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C125" s="123" t="s">
+      <c r="C125" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E125" s="4" t="s">
@@ -15630,7 +15630,7 @@
       <c r="B126" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C126" s="123" t="s">
+      <c r="C126" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E126" s="4" t="s">
@@ -15650,7 +15650,7 @@
       <c r="B127" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C127" s="123" t="s">
+      <c r="C127" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E127" s="4" t="s">
@@ -15670,7 +15670,7 @@
       <c r="B128" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C128" s="123" t="s">
+      <c r="C128" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E128" s="4" t="s">
@@ -15690,7 +15690,7 @@
       <c r="B129" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C129" s="123" t="s">
+      <c r="C129" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E129" s="4" t="s">
@@ -15710,7 +15710,7 @@
       <c r="B130" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C130" s="123" t="s">
+      <c r="C130" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E130" s="4" t="s">
@@ -15730,7 +15730,7 @@
       <c r="B131" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C131" s="123" t="s">
+      <c r="C131" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E131" s="4" t="s">
@@ -15750,7 +15750,7 @@
       <c r="B132" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C132" s="123" t="s">
+      <c r="C132" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E132" s="4" t="s">
@@ -15770,7 +15770,7 @@
       <c r="B133" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C133" s="123" t="s">
+      <c r="C133" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E133" s="4" t="s">
@@ -15790,7 +15790,7 @@
       <c r="B134" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C134" s="123" t="s">
+      <c r="C134" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E134" s="4" t="s">
@@ -15810,7 +15810,7 @@
       <c r="B135" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C135" s="123" t="s">
+      <c r="C135" s="121" t="s">
         <v>657</v>
       </c>
       <c r="E135" s="4" t="s">
@@ -16967,31 +16967,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="68" customFormat="1" ht="15.75">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>308</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
-      <c r="O1" s="122"/>
-      <c r="P1" s="122"/>
-      <c r="Q1" s="122"/>
-      <c r="R1" s="122"/>
-      <c r="S1" s="122"/>
-      <c r="T1" s="122"/>
-      <c r="U1" s="122"/>
-      <c r="V1" s="122"/>
-      <c r="W1" s="122"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="123"/>
+      <c r="S1" s="123"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="123"/>
+      <c r="V1" s="123"/>
+      <c r="W1" s="123"/>
       <c r="X1" s="95"/>
     </row>
     <row r="2" spans="1:24" ht="13.15">

</xml_diff>